<commit_message>
feat: page resultforTest, second test logic
</commit_message>
<xml_diff>
--- a/public/course-data.xlsx
+++ b/public/course-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Root\Desktop\test\SEAL-project\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38E89FB-10D5-45FB-A969-24B4F0E4B37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF7C55A-9098-4FCB-8501-04962E45EBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4641B334-F7E7-45C7-AC33-35F16097774F}"/>
+    <workbookView xWindow="825" yWindow="3945" windowWidth="14835" windowHeight="10965" xr2:uid="{4641B334-F7E7-45C7-AC33-35F16097774F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>과정1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,6 +59,30 @@
   </si>
   <si>
     <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\Users\Root\Desktop\test\SEAL-project\src\assets\logos\logo1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\Users\Root\Desktop\test\SEAL-project\src\assets\logos\logo2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\Users\Root\Desktop\test\SEAL-project\src\assets\logos\logo3.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\Users\Root\Desktop\test\SEAL-project\src\assets\logos\logo4.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\Users\Root\Desktop\test\SEAL-project\src\assets\logos\logo5.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -443,43 +467,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBF5C87-7A95-4471-8A9E-10835A9C23DF}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="2" max="2" width="64.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>